<commit_message>
latest edits to code
elasticities work out for LC model but not for PY model with het. Next add code changes to paper and slides
</commit_message>
<xml_diff>
--- a/Results/Lorenz_by_age_LCrrDistNetWorth.xlsx
+++ b/Results/Lorenz_by_age_LCrrDistNetWorth.xlsx
@@ -462,16 +462,16 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>-0.0001868547545534963</v>
+        <v>-0.004282840336034826</v>
       </c>
       <c r="C2">
-        <v>0.03047356714340979</v>
+        <v>0.02302100293418834</v>
       </c>
       <c r="D2">
-        <v>0.1005458947508881</v>
+        <v>0.08579924713921762</v>
       </c>
       <c r="E2">
-        <v>0.2532346143786333</v>
+        <v>0.22516039235143</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -479,16 +479,16 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>-0.008609052404084341</v>
+        <v>-0.01855104846907478</v>
       </c>
       <c r="C3">
-        <v>0.01776568585415393</v>
+        <v>0.005422169068455969</v>
       </c>
       <c r="D3">
-        <v>0.09471479682996145</v>
+        <v>0.07479120730010015</v>
       </c>
       <c r="E3">
-        <v>0.2730039994266019</v>
+        <v>0.2378289229639267</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -496,16 +496,16 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>-0.01114052884754069</v>
+        <v>-0.02613736430319635</v>
       </c>
       <c r="C4">
-        <v>0.008571963747890543</v>
+        <v>-0.007154220427063259</v>
       </c>
       <c r="D4">
-        <v>0.08064164729195009</v>
+        <v>0.05967910789027422</v>
       </c>
       <c r="E4">
-        <v>0.2636468948719055</v>
+        <v>0.2305681723758092</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -513,16 +513,16 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>-0.007728730505176792</v>
+        <v>-0.01955700770304824</v>
       </c>
       <c r="C5">
-        <v>0.009471882603127025</v>
+        <v>-0.001125629226679811</v>
       </c>
       <c r="D5">
-        <v>0.07789363271128716</v>
+        <v>0.06478498766028414</v>
       </c>
       <c r="E5">
-        <v>0.2600061436942636</v>
+        <v>0.2380158442442341</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -530,16 +530,16 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>-0.003129687019554217</v>
+        <v>-0.00854105973134241</v>
       </c>
       <c r="C6">
-        <v>0.01467343829663756</v>
+        <v>0.01318274608469809</v>
       </c>
       <c r="D6">
-        <v>0.08180780472419802</v>
+        <v>0.08160447448843923</v>
       </c>
       <c r="E6">
-        <v>0.2611205721742703</v>
+        <v>0.255838728315701</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -547,16 +547,16 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>0.0003170317622659856</v>
+        <v>-6.230550227516185E-05</v>
       </c>
       <c r="C7">
-        <v>0.01972197010722334</v>
+        <v>0.02619313379369959</v>
       </c>
       <c r="D7">
-        <v>0.08635937120965467</v>
+        <v>0.09844080080017134</v>
       </c>
       <c r="E7">
-        <v>0.2621863319619264</v>
+        <v>0.2726153113653246</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -564,16 +564,16 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>0.001962041621723962</v>
+        <v>0.004033704328844627</v>
       </c>
       <c r="C8">
-        <v>0.02237057962160435</v>
+        <v>0.03322454103344932</v>
       </c>
       <c r="D8">
-        <v>0.08797995699963443</v>
+        <v>0.1078608596092078</v>
       </c>
       <c r="E8">
-        <v>0.2600362839403036</v>
+        <v>0.2812938098090068</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -581,16 +581,16 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>0.002980050080565763</v>
+        <v>0.006306681806613115</v>
       </c>
       <c r="C9">
-        <v>0.02397804994533067</v>
+        <v>0.03761272248300324</v>
       </c>
       <c r="D9">
-        <v>0.08810811189932835</v>
+        <v>0.1133327832638251</v>
       </c>
       <c r="E9">
-        <v>0.2561973791226438</v>
+        <v>0.2853922200211083</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -598,16 +598,16 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <v>0.0002529031770905285</v>
+        <v>0.001343701675643187</v>
       </c>
       <c r="C10">
-        <v>0.01661624943206456</v>
+        <v>0.02707462818091589</v>
       </c>
       <c r="D10">
-        <v>0.07382796959075368</v>
+        <v>0.09615231592399624</v>
       </c>
       <c r="E10">
-        <v>0.235527327725442</v>
+        <v>0.2628644012402884</v>
       </c>
     </row>
   </sheetData>
@@ -645,16 +645,16 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>-0.0001868547545534963</v>
+        <v>-0.004282840336034826</v>
       </c>
       <c r="C2">
-        <v>0.03047356714340979</v>
+        <v>0.02302100293418834</v>
       </c>
       <c r="D2">
-        <v>0.1005458947508881</v>
+        <v>0.08579924713921762</v>
       </c>
       <c r="E2">
-        <v>0.2532346143786333</v>
+        <v>0.22516039235143</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -662,16 +662,16 @@
         <v>14</v>
       </c>
       <c r="B3">
-        <v>-0.01010619226149713</v>
+        <v>-0.0226730292340869</v>
       </c>
       <c r="C3">
-        <v>0.01215886996185689</v>
+        <v>-0.001373785615127518</v>
       </c>
       <c r="D3">
-        <v>0.08409717121145673</v>
+        <v>0.0659747206858326</v>
       </c>
       <c r="E3">
-        <v>0.2608807519784946</v>
+        <v>0.2316682306050966</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -679,16 +679,16 @@
         <v>15</v>
       </c>
       <c r="B4">
-        <v>-0.005171609681374163</v>
+        <v>-0.01353279462471494</v>
       </c>
       <c r="C4">
-        <v>0.01207790644405074</v>
+        <v>0.006319617599752947</v>
       </c>
       <c r="D4">
-        <v>0.07865006300258831</v>
+        <v>0.07269332730951769</v>
       </c>
       <c r="E4">
-        <v>0.2569327862415205</v>
+        <v>0.2450556704557504</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -696,16 +696,16 @@
         <v>16</v>
       </c>
       <c r="B5">
-        <v>0.001137601516994725</v>
+        <v>0.001959036517865503</v>
       </c>
       <c r="C5">
-        <v>0.02090725041232334</v>
+        <v>0.02945572141998663</v>
       </c>
       <c r="D5">
-        <v>0.08655368420975317</v>
+        <v>0.1025130401938906</v>
       </c>
       <c r="E5">
-        <v>0.2592784568451815</v>
+        <v>0.2757024079197318</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -713,16 +713,16 @@
         <v>17</v>
       </c>
       <c r="B6">
-        <v>0.001573758507314009</v>
+        <v>0.003841510628239411</v>
       </c>
       <c r="C6">
-        <v>0.02030668986249531</v>
+        <v>0.03250357040539691</v>
       </c>
       <c r="D6">
-        <v>0.08106103290982179</v>
+        <v>0.1051671806429676</v>
       </c>
       <c r="E6">
-        <v>0.2458943385163051</v>
+        <v>0.2748122718004537</v>
       </c>
     </row>
   </sheetData>

</xml_diff>